<commit_message>
Completed reading data on all variables
</commit_message>
<xml_diff>
--- a/public/MADISON-BETTERLIFE-SME-RATE-CARD.xlsx
+++ b/public/MADISON-BETTERLIFE-SME-RATE-CARD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paul.kamau\Desktop\app-test\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paul.kamau\Desktop\Madison BetterLife\my-app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2BD14FD-4C02-4382-8BBF-1CCD94FD9AEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2FEE3F7-D8DE-4669-8A9E-E88024173C05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9525" windowHeight="7890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9525" windowHeight="7890" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InpatientAbove18" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="18">
   <si>
     <t>A</t>
   </si>
@@ -96,56 +96,66 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color rgb="FFFFFFFF"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color rgb="FFFF0000"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FFFF0000"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -275,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
@@ -331,9 +341,6 @@
     <xf numFmtId="3" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
     <xf numFmtId="3" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
@@ -653,7 +660,7 @@
   </sheetPr>
   <dimension ref="A1:AL66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
@@ -3620,10 +3627,10 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3634,184 +3641,169 @@
     <col min="9" max="10" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="36" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="13" t="s">
+    <row r="1" spans="1:9" s="35" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="B1" s="34" t="s">
         <v>9</v>
       </c>
+      <c r="C1" s="16" t="s">
+        <v>10</v>
+      </c>
       <c r="D1" s="16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="19" customFormat="1" ht="14.25" collapsed="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:9" s="19" customFormat="1" ht="14.25" collapsed="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="17">
+        <v>250000</v>
+      </c>
+      <c r="B2" s="15">
+        <v>54600</v>
+      </c>
+      <c r="C2" s="15">
+        <v>65520</v>
+      </c>
+      <c r="D2" s="15">
+        <v>76440</v>
+      </c>
+      <c r="E2" s="15">
+        <v>87360</v>
+      </c>
+      <c r="F2" s="15">
+        <v>98280</v>
+      </c>
+      <c r="G2" s="15">
+        <v>109200</v>
+      </c>
+      <c r="H2" s="15">
+        <v>120120</v>
+      </c>
+      <c r="I2" s="15">
         <v>0</v>
       </c>
-      <c r="B2" s="17">
-        <v>250000</v>
-      </c>
-      <c r="C2" s="15">
-        <v>54600</v>
-      </c>
-      <c r="D2" s="15">
-        <v>65520</v>
-      </c>
-      <c r="E2" s="15">
-        <v>76440</v>
-      </c>
-      <c r="F2" s="15">
-        <v>87360</v>
-      </c>
-      <c r="G2" s="15">
-        <v>98280</v>
-      </c>
-      <c r="H2" s="15">
-        <v>109200</v>
-      </c>
-      <c r="I2" s="15">
-        <v>120120</v>
-      </c>
-      <c r="J2" s="15">
+    </row>
+    <row r="3" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17">
+        <v>200000</v>
+      </c>
+      <c r="B3" s="15">
+        <v>45600</v>
+      </c>
+      <c r="C3" s="15">
+        <v>56520</v>
+      </c>
+      <c r="D3" s="15">
+        <v>67440</v>
+      </c>
+      <c r="E3" s="15">
+        <v>78360</v>
+      </c>
+      <c r="F3" s="15">
+        <v>89280</v>
+      </c>
+      <c r="G3" s="15">
+        <v>100200</v>
+      </c>
+      <c r="H3" s="15">
+        <v>111120</v>
+      </c>
+      <c r="I3" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="17">
-        <v>200000</v>
-      </c>
-      <c r="C3" s="15">
-        <v>45600</v>
-      </c>
-      <c r="D3" s="15">
-        <v>56520</v>
-      </c>
-      <c r="E3" s="15">
-        <v>67440</v>
-      </c>
-      <c r="F3" s="15">
-        <v>78360</v>
-      </c>
-      <c r="G3" s="15">
-        <v>89280</v>
-      </c>
-      <c r="H3" s="15">
-        <v>100200</v>
-      </c>
-      <c r="I3" s="15">
-        <v>111120</v>
-      </c>
-      <c r="J3" s="15">
+    <row r="4" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
+        <v>150000</v>
+      </c>
+      <c r="B4" s="15">
+        <v>36600</v>
+      </c>
+      <c r="C4" s="15">
+        <v>47520</v>
+      </c>
+      <c r="D4" s="15">
+        <v>58440</v>
+      </c>
+      <c r="E4" s="15">
+        <v>69360</v>
+      </c>
+      <c r="F4" s="15">
+        <v>80280</v>
+      </c>
+      <c r="G4" s="15">
+        <v>91200</v>
+      </c>
+      <c r="H4" s="15">
+        <v>102120</v>
+      </c>
+      <c r="I4" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="17">
-        <v>150000</v>
-      </c>
-      <c r="C4" s="15">
-        <v>36600</v>
-      </c>
-      <c r="D4" s="15">
-        <v>47520</v>
-      </c>
-      <c r="E4" s="15">
-        <v>58440</v>
-      </c>
-      <c r="F4" s="15">
-        <v>69360</v>
-      </c>
-      <c r="G4" s="15">
-        <v>80280</v>
-      </c>
-      <c r="H4" s="15">
-        <v>91200</v>
-      </c>
-      <c r="I4" s="15">
-        <v>102120</v>
-      </c>
-      <c r="J4" s="15">
+    <row r="5" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
+        <v>100000</v>
+      </c>
+      <c r="B5" s="15">
+        <v>27600</v>
+      </c>
+      <c r="C5" s="15">
+        <v>38520</v>
+      </c>
+      <c r="D5" s="15">
+        <v>49440</v>
+      </c>
+      <c r="E5" s="15">
+        <v>60360</v>
+      </c>
+      <c r="F5" s="15">
+        <v>71280</v>
+      </c>
+      <c r="G5" s="15">
+        <v>82200</v>
+      </c>
+      <c r="H5" s="15">
+        <v>93120</v>
+      </c>
+      <c r="I5" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="17">
-        <v>100000</v>
-      </c>
-      <c r="C5" s="15">
-        <v>27600</v>
-      </c>
-      <c r="D5" s="15">
-        <v>38520</v>
-      </c>
-      <c r="E5" s="15">
-        <v>49440</v>
-      </c>
-      <c r="F5" s="15">
-        <v>60360</v>
-      </c>
-      <c r="G5" s="15">
-        <v>71280</v>
-      </c>
-      <c r="H5" s="15">
-        <v>82200</v>
-      </c>
-      <c r="I5" s="15">
-        <v>93120</v>
-      </c>
-      <c r="J5" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="17">
+    <row r="6" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
         <v>75000</v>
       </c>
+      <c r="B6" s="15">
+        <v>23100</v>
+      </c>
       <c r="C6" s="15">
-        <v>23100</v>
+        <v>34020</v>
       </c>
       <c r="D6" s="15">
-        <v>34020</v>
+        <v>44940</v>
       </c>
       <c r="E6" s="15">
-        <v>44940</v>
+        <v>55860</v>
       </c>
       <c r="F6" s="15">
-        <v>55860</v>
+        <v>66780</v>
       </c>
       <c r="G6" s="15">
         <v>66780</v>
@@ -3820,24 +3812,21 @@
         <v>66780</v>
       </c>
       <c r="I6" s="15">
-        <v>66780</v>
-      </c>
-      <c r="J6" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="17">
+    <row r="7" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
         <v>50000</v>
       </c>
+      <c r="B7" s="15">
+        <v>18600</v>
+      </c>
       <c r="C7" s="15">
-        <v>18600</v>
+        <v>29520</v>
       </c>
       <c r="D7" s="15">
-        <v>29520</v>
+        <v>40440</v>
       </c>
       <c r="E7" s="15">
         <v>40440</v>
@@ -3852,24 +3841,21 @@
         <v>40440</v>
       </c>
       <c r="I7" s="15">
-        <v>40440</v>
-      </c>
-      <c r="J7" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="17">
+    <row r="8" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17">
         <v>40000</v>
       </c>
+      <c r="B8" s="15">
+        <v>16800</v>
+      </c>
       <c r="C8" s="15">
-        <v>16800</v>
+        <v>27720</v>
       </c>
       <c r="D8" s="15">
-        <v>27720</v>
+        <v>38640</v>
       </c>
       <c r="E8" s="15">
         <v>38640</v>
@@ -3884,13 +3870,10 @@
         <v>38640</v>
       </c>
       <c r="I8" s="15">
-        <v>38640</v>
-      </c>
-      <c r="J8" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9"/>
@@ -3900,7 +3883,7 @@
       <c r="G9"/>
       <c r="H9"/>
     </row>
-    <row r="10" spans="1:10" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
@@ -3910,7 +3893,7 @@
       <c r="G10"/>
       <c r="H10"/>
     </row>
-    <row r="11" spans="1:10" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
@@ -3920,7 +3903,7 @@
       <c r="G11"/>
       <c r="H11"/>
     </row>
-    <row r="12" spans="1:10" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
@@ -3930,7 +3913,7 @@
       <c r="G12"/>
       <c r="H12"/>
     </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
@@ -3940,7 +3923,7 @@
       <c r="G13"/>
       <c r="H13"/>
     </row>
-    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
@@ -3950,7 +3933,7 @@
       <c r="G14"/>
       <c r="H14"/>
     </row>
-    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
@@ -3960,7 +3943,7 @@
       <c r="G15"/>
       <c r="H15"/>
     </row>
-    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
@@ -4011,13 +3994,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="36" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="16" t="s">
@@ -4278,8 +4261,8 @@
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4296,240 +4279,249 @@
       <c r="A1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="21">
+      <c r="B1" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="12"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="21">
         <v>10000</v>
-      </c>
-      <c r="C1" s="20">
-        <v>20000</v>
-      </c>
-      <c r="D1" s="20">
-        <v>25000</v>
-      </c>
-      <c r="E1" s="20">
-        <v>30000</v>
-      </c>
-      <c r="F1" s="20">
-        <v>35000</v>
-      </c>
-      <c r="G1" s="20">
-        <v>40000</v>
-      </c>
-      <c r="H1" s="20">
-        <v>45000</v>
-      </c>
-      <c r="I1" s="20">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
-        <v>9</v>
       </c>
       <c r="B2" s="23">
         <v>3250</v>
       </c>
       <c r="C2" s="23">
+        <v>4250</v>
+      </c>
+      <c r="D2" s="23">
+        <v>4750</v>
+      </c>
+      <c r="E2" s="23">
+        <v>5250</v>
+      </c>
+      <c r="F2" s="23">
+        <v>5750</v>
+      </c>
+      <c r="G2" s="23">
+        <v>6750</v>
+      </c>
+      <c r="H2" s="25">
+        <v>1012.5</v>
+      </c>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="20">
+        <v>20000</v>
+      </c>
+      <c r="B3" s="23">
         <v>6500</v>
-      </c>
-      <c r="D2" s="23">
-        <v>8125</v>
-      </c>
-      <c r="E2" s="23">
-        <v>9750</v>
-      </c>
-      <c r="F2" s="23">
-        <v>11375</v>
-      </c>
-      <c r="G2" s="23">
-        <v>13000</v>
-      </c>
-      <c r="H2" s="23">
-        <v>14625</v>
-      </c>
-      <c r="I2" s="23">
-        <v>16250</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="23">
-        <v>4250</v>
       </c>
       <c r="C3" s="23">
         <v>8500</v>
       </c>
       <c r="D3" s="23">
+        <v>9500</v>
+      </c>
+      <c r="E3" s="23">
+        <v>10500</v>
+      </c>
+      <c r="F3" s="23">
+        <v>11500</v>
+      </c>
+      <c r="G3" s="23">
+        <v>13500</v>
+      </c>
+      <c r="H3" s="25">
+        <v>2025</v>
+      </c>
+      <c r="I3" s="12"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="20">
+        <v>25000</v>
+      </c>
+      <c r="B4" s="23">
+        <v>8125</v>
+      </c>
+      <c r="C4" s="23">
         <v>10625</v>
-      </c>
-      <c r="E3" s="23">
-        <v>12750</v>
-      </c>
-      <c r="F3" s="23">
-        <v>14875</v>
-      </c>
-      <c r="G3" s="23">
-        <v>17000</v>
-      </c>
-      <c r="H3" s="23">
-        <v>19125</v>
-      </c>
-      <c r="I3" s="23">
-        <v>21250</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="23">
-        <v>4750</v>
-      </c>
-      <c r="C4" s="23">
-        <v>9500</v>
       </c>
       <c r="D4" s="23">
         <v>11875</v>
       </c>
       <c r="E4" s="23">
+        <v>13125</v>
+      </c>
+      <c r="F4" s="23">
+        <v>14375</v>
+      </c>
+      <c r="G4" s="23">
+        <v>16875</v>
+      </c>
+      <c r="H4" s="25">
+        <v>2531.25</v>
+      </c>
+      <c r="I4" s="12"/>
+      <c r="L4" s="33"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="20">
+        <v>30000</v>
+      </c>
+      <c r="B5" s="23">
+        <v>9750</v>
+      </c>
+      <c r="C5" s="23">
+        <v>12750</v>
+      </c>
+      <c r="D5" s="23">
         <v>14250</v>
-      </c>
-      <c r="F4" s="23">
-        <v>16625</v>
-      </c>
-      <c r="G4" s="23">
-        <v>19000</v>
-      </c>
-      <c r="H4" s="23">
-        <v>21375</v>
-      </c>
-      <c r="I4" s="23">
-        <v>23750</v>
-      </c>
-      <c r="L4" s="33"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="23">
-        <v>5250</v>
-      </c>
-      <c r="C5" s="23">
-        <v>10500</v>
-      </c>
-      <c r="D5" s="23">
-        <v>13125</v>
       </c>
       <c r="E5" s="23">
         <v>15750</v>
       </c>
       <c r="F5" s="23">
+        <v>17250</v>
+      </c>
+      <c r="G5" s="23">
+        <v>20250</v>
+      </c>
+      <c r="H5" s="25">
+        <v>3037.5</v>
+      </c>
+      <c r="I5" s="12"/>
+      <c r="L5" s="33"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="20">
+        <v>35000</v>
+      </c>
+      <c r="B6" s="23">
+        <v>11375</v>
+      </c>
+      <c r="C6" s="23">
+        <v>14875</v>
+      </c>
+      <c r="D6" s="23">
+        <v>16625</v>
+      </c>
+      <c r="E6" s="23">
         <v>18375</v>
-      </c>
-      <c r="G5" s="23">
-        <v>21000</v>
-      </c>
-      <c r="H5" s="23">
-        <v>23625</v>
-      </c>
-      <c r="I5" s="23">
-        <v>26250</v>
-      </c>
-      <c r="L5" s="33"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="23">
-        <v>5750</v>
-      </c>
-      <c r="C6" s="23">
-        <v>11500</v>
-      </c>
-      <c r="D6" s="23">
-        <v>14375</v>
-      </c>
-      <c r="E6" s="23">
-        <v>17250</v>
       </c>
       <c r="F6" s="23">
         <v>20125</v>
       </c>
       <c r="G6" s="23">
+        <v>23625</v>
+      </c>
+      <c r="H6" s="25">
+        <v>3543.75</v>
+      </c>
+      <c r="I6" s="12"/>
+      <c r="L6" s="33"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="20">
+        <v>40000</v>
+      </c>
+      <c r="B7" s="23">
+        <v>13000</v>
+      </c>
+      <c r="C7" s="23">
+        <v>17000</v>
+      </c>
+      <c r="D7" s="23">
+        <v>19000</v>
+      </c>
+      <c r="E7" s="23">
+        <v>21000</v>
+      </c>
+      <c r="F7" s="23">
         <v>23000</v>
-      </c>
-      <c r="H6" s="23">
-        <v>25875</v>
-      </c>
-      <c r="I6" s="23">
-        <v>28750</v>
-      </c>
-      <c r="L6" s="33"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="23">
-        <v>6750</v>
-      </c>
-      <c r="C7" s="23">
-        <v>13500</v>
-      </c>
-      <c r="D7" s="23">
-        <v>16875</v>
-      </c>
-      <c r="E7" s="23">
-        <v>20250</v>
-      </c>
-      <c r="F7" s="23">
-        <v>23625</v>
       </c>
       <c r="G7" s="23">
         <v>27000</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="25">
+        <v>4050</v>
+      </c>
+      <c r="I7" s="12"/>
+      <c r="L7" s="33"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="20">
+        <v>45000</v>
+      </c>
+      <c r="B8" s="23">
+        <v>14625</v>
+      </c>
+      <c r="C8" s="23">
+        <v>19125</v>
+      </c>
+      <c r="D8" s="23">
+        <v>21375</v>
+      </c>
+      <c r="E8" s="23">
+        <v>23625</v>
+      </c>
+      <c r="F8" s="23">
+        <v>25875</v>
+      </c>
+      <c r="G8" s="23">
         <v>30375</v>
-      </c>
-      <c r="I7" s="23">
-        <v>33750</v>
-      </c>
-      <c r="L7" s="33"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="25">
-        <v>1012.5</v>
-      </c>
-      <c r="C8" s="25">
-        <v>2025</v>
-      </c>
-      <c r="D8" s="25">
-        <v>2531.25</v>
-      </c>
-      <c r="E8" s="25">
-        <v>3037.5</v>
-      </c>
-      <c r="F8" s="25">
-        <v>3543.75</v>
-      </c>
-      <c r="G8" s="25">
-        <v>4050</v>
       </c>
       <c r="H8" s="25">
         <v>4556.25</v>
       </c>
-      <c r="I8" s="25">
+      <c r="I8" s="12"/>
+      <c r="L8" s="33"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="20">
+        <v>50000</v>
+      </c>
+      <c r="B9" s="23">
+        <v>16250</v>
+      </c>
+      <c r="C9" s="23">
+        <v>21250</v>
+      </c>
+      <c r="D9" s="23">
+        <v>23750</v>
+      </c>
+      <c r="E9" s="23">
+        <v>26250</v>
+      </c>
+      <c r="F9" s="23">
+        <v>28750</v>
+      </c>
+      <c r="G9" s="23">
+        <v>33750</v>
+      </c>
+      <c r="H9" s="25">
         <v>5062.5</v>
       </c>
-      <c r="L8" s="33"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I9" s="12"/>
       <c r="L9" s="33"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modified the Fetching ,ethod to include check for age variable.
</commit_message>
<xml_diff>
--- a/public/MADISON-BETTERLIFE-SME-RATE-CARD.xlsx
+++ b/public/MADISON-BETTERLIFE-SME-RATE-CARD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paul.kamau\Desktop\Madison BetterLife\my-app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2FEE3F7-D8DE-4669-8A9E-E88024173C05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39B8E21-0D56-4A9D-8589-452E9A899554}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9525" windowHeight="7890" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9525" windowHeight="7890" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InpatientAbove18" sheetId="3" r:id="rId1"/>
@@ -26,31 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="18">
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>Option</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="10">
   <si>
     <t>Limit</t>
   </si>
@@ -221,7 +197,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -258,19 +234,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -285,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
@@ -302,9 +265,6 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="3" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -340,13 +300,10 @@
     <xf numFmtId="3" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="3" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
-    <xf numFmtId="3" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="3" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -681,60 +638,60 @@
   <sheetData>
     <row r="1" spans="1:38" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:38" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32">
+      <c r="A2" s="31">
         <v>5000000</v>
       </c>
-      <c r="B2" s="31">
+      <c r="B2" s="30">
         <v>44500</v>
       </c>
-      <c r="C2" s="31">
+      <c r="C2" s="30">
         <v>62300</v>
       </c>
-      <c r="D2" s="31">
+      <c r="D2" s="30">
         <v>80100</v>
       </c>
-      <c r="E2" s="31">
+      <c r="E2" s="30">
         <v>97900</v>
       </c>
-      <c r="F2" s="31">
+      <c r="F2" s="30">
         <v>115700</v>
       </c>
-      <c r="G2" s="31">
+      <c r="G2" s="30">
         <v>133500</v>
       </c>
-      <c r="H2" s="31">
+      <c r="H2" s="30">
         <v>151300</v>
       </c>
-      <c r="I2" s="31"/>
+      <c r="I2" s="30"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -765,31 +722,31 @@
       <c r="AK2" s="1"/>
     </row>
     <row r="3" spans="1:38" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32">
+      <c r="A3" s="31">
         <v>3000000</v>
       </c>
-      <c r="B3" s="31">
+      <c r="B3" s="30">
         <v>38500</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="30">
         <v>53900</v>
       </c>
-      <c r="D3" s="31">
+      <c r="D3" s="30">
         <v>69300</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="30">
         <v>84700</v>
       </c>
-      <c r="F3" s="31">
+      <c r="F3" s="30">
         <v>100100</v>
       </c>
-      <c r="G3" s="31">
+      <c r="G3" s="30">
         <v>117900</v>
       </c>
-      <c r="H3" s="31">
+      <c r="H3" s="30">
         <v>135700</v>
       </c>
-      <c r="I3" s="31"/>
+      <c r="I3" s="30"/>
       <c r="J3" s="2"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -820,31 +777,31 @@
       <c r="AK3" s="1"/>
     </row>
     <row r="4" spans="1:38" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32">
+      <c r="A4" s="31">
         <v>2500000</v>
       </c>
-      <c r="B4" s="31">
+      <c r="B4" s="30">
         <v>37000</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="30">
         <v>51800</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="30">
         <v>66600</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="30">
         <v>81400</v>
       </c>
-      <c r="F4" s="31">
+      <c r="F4" s="30">
         <v>96200</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G4" s="30">
         <v>111000</v>
       </c>
-      <c r="H4" s="31">
+      <c r="H4" s="30">
         <v>125800</v>
       </c>
-      <c r="I4" s="31"/>
+      <c r="I4" s="30"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -875,31 +832,31 @@
       <c r="AK4" s="2"/>
     </row>
     <row r="5" spans="1:38" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32">
+      <c r="A5" s="31">
         <v>2000000</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="30">
         <v>32000</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="30">
         <v>44800</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="30">
         <v>57600</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="30">
         <v>70400</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="30">
         <v>83200</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="30">
         <v>96000</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="30">
         <v>108800</v>
       </c>
-      <c r="I5" s="31"/>
+      <c r="I5" s="30"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -930,31 +887,31 @@
       <c r="AK5" s="2"/>
     </row>
     <row r="6" spans="1:38" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="32">
+      <c r="A6" s="31">
         <v>1500000</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="30">
         <v>27000</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="30">
         <v>37800</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="30">
         <v>48600</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E6" s="30">
         <v>59400</v>
       </c>
-      <c r="F6" s="31">
+      <c r="F6" s="30">
         <v>70200</v>
       </c>
-      <c r="G6" s="31">
+      <c r="G6" s="30">
         <v>81000</v>
       </c>
-      <c r="H6" s="31">
+      <c r="H6" s="30">
         <v>91800</v>
       </c>
-      <c r="I6" s="31"/>
+      <c r="I6" s="30"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -985,31 +942,31 @@
       <c r="AK6" s="2"/>
     </row>
     <row r="7" spans="1:38" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32">
+      <c r="A7" s="31">
         <v>1000000</v>
       </c>
-      <c r="B7" s="31">
+      <c r="B7" s="30">
         <v>22000</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="30">
         <v>30800</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="30">
         <v>39600</v>
       </c>
-      <c r="E7" s="31">
+      <c r="E7" s="30">
         <v>48400</v>
       </c>
-      <c r="F7" s="31">
+      <c r="F7" s="30">
         <v>57200</v>
       </c>
-      <c r="G7" s="31">
+      <c r="G7" s="30">
         <v>66000</v>
       </c>
-      <c r="H7" s="31">
+      <c r="H7" s="30">
         <v>74800</v>
       </c>
-      <c r="I7" s="31"/>
+      <c r="I7" s="30"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -1040,31 +997,31 @@
       <c r="AK7" s="2"/>
     </row>
     <row r="8" spans="1:38" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32">
+      <c r="A8" s="31">
         <v>750000</v>
       </c>
-      <c r="B8" s="31">
+      <c r="B8" s="30">
         <v>19500</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="30">
         <v>27300</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="30">
         <v>35100</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="30">
         <v>42900</v>
       </c>
-      <c r="F8" s="31">
+      <c r="F8" s="30">
         <v>50700</v>
       </c>
-      <c r="G8" s="31">
+      <c r="G8" s="30">
         <v>58500</v>
       </c>
-      <c r="H8" s="31">
+      <c r="H8" s="30">
         <v>66300</v>
       </c>
-      <c r="I8" s="31"/>
+      <c r="I8" s="30"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -1095,31 +1052,31 @@
       <c r="AK8" s="2"/>
     </row>
     <row r="9" spans="1:38" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="32">
+      <c r="A9" s="31">
         <v>500000</v>
       </c>
-      <c r="B9" s="31">
+      <c r="B9" s="30">
         <v>17000</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="30">
         <v>23800</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="30">
         <v>30600</v>
       </c>
-      <c r="E9" s="31">
+      <c r="E9" s="30">
         <v>37400</v>
       </c>
-      <c r="F9" s="31">
+      <c r="F9" s="30">
         <v>44200</v>
       </c>
-      <c r="G9" s="31">
+      <c r="G9" s="30">
         <v>51000</v>
       </c>
-      <c r="H9" s="31">
+      <c r="H9" s="30">
         <v>57800</v>
       </c>
-      <c r="I9" s="31"/>
+      <c r="I9" s="30"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -1150,31 +1107,31 @@
       <c r="AK9" s="2"/>
     </row>
     <row r="10" spans="1:38" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32">
+      <c r="A10" s="31">
         <v>300000</v>
       </c>
-      <c r="B10" s="31">
+      <c r="B10" s="30">
         <v>15000</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="30">
         <v>21000</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="30">
         <v>27000</v>
       </c>
-      <c r="E10" s="31">
+      <c r="E10" s="30">
         <v>33000</v>
       </c>
-      <c r="F10" s="31">
+      <c r="F10" s="30">
         <v>39000</v>
       </c>
-      <c r="G10" s="31">
+      <c r="G10" s="30">
         <v>45000</v>
       </c>
-      <c r="H10" s="31">
+      <c r="H10" s="30">
         <v>51000</v>
       </c>
-      <c r="I10" s="31"/>
+      <c r="I10" s="30"/>
       <c r="J10" s="4"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -1205,31 +1162,31 @@
       <c r="AK10" s="2"/>
     </row>
     <row r="11" spans="1:38" s="12" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32">
+      <c r="A11" s="31">
         <v>200000</v>
       </c>
-      <c r="B11" s="31">
+      <c r="B11" s="30">
         <v>14000</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="30">
         <v>19600</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="30">
         <v>25200</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E11" s="30">
         <v>30800</v>
       </c>
-      <c r="F11" s="31">
+      <c r="F11" s="30">
         <v>36400</v>
       </c>
-      <c r="G11" s="31">
+      <c r="G11" s="30">
         <v>42000</v>
       </c>
-      <c r="H11" s="31">
+      <c r="H11" s="30">
         <v>47600</v>
       </c>
-      <c r="I11" s="31"/>
+      <c r="I11" s="30"/>
       <c r="J11" s="2"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
@@ -1269,7 +1226,7 @@
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
-      <c r="J12" s="29"/>
+      <c r="J12" s="28"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -1298,7 +1255,7 @@
       <c r="AJ12" s="2"/>
       <c r="AK12" s="2"/>
     </row>
-    <row r="13" spans="1:38" s="30" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" s="29" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1309,33 +1266,33 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="29"/>
-      <c r="R13" s="29"/>
-      <c r="S13" s="29"/>
-      <c r="T13" s="29"/>
-      <c r="U13" s="29"/>
-      <c r="V13" s="29"/>
-      <c r="W13" s="29"/>
-      <c r="X13" s="29"/>
-      <c r="Y13" s="29"/>
-      <c r="Z13" s="29"/>
-      <c r="AA13" s="29"/>
-      <c r="AB13" s="29"/>
-      <c r="AC13" s="29"/>
-      <c r="AD13" s="29"/>
-      <c r="AE13" s="29"/>
-      <c r="AF13" s="29"/>
-      <c r="AG13" s="29"/>
-      <c r="AH13" s="29"/>
-      <c r="AI13" s="29"/>
-      <c r="AJ13" s="29"/>
-      <c r="AK13" s="29"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="28"/>
+      <c r="S13" s="28"/>
+      <c r="T13" s="28"/>
+      <c r="U13" s="28"/>
+      <c r="V13" s="28"/>
+      <c r="W13" s="28"/>
+      <c r="X13" s="28"/>
+      <c r="Y13" s="28"/>
+      <c r="Z13" s="28"/>
+      <c r="AA13" s="28"/>
+      <c r="AB13" s="28"/>
+      <c r="AC13" s="28"/>
+      <c r="AD13" s="28"/>
+      <c r="AE13" s="28"/>
+      <c r="AF13" s="28"/>
+      <c r="AG13" s="28"/>
+      <c r="AH13" s="28"/>
+      <c r="AI13" s="28"/>
+      <c r="AJ13" s="28"/>
+      <c r="AK13" s="28"/>
     </row>
     <row r="14" spans="1:38" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -3300,59 +3257,59 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="13" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>5000000</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="14">
         <v>53400</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="14">
         <v>74760</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="14">
         <v>96120</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="14">
         <v>117480</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="14">
         <v>138840</v>
       </c>
-      <c r="G2" s="15">
+      <c r="G2" s="14">
         <v>160200</v>
       </c>
-      <c r="H2" s="15">
+      <c r="H2" s="14">
         <v>181560</v>
       </c>
-      <c r="I2" s="15">
+      <c r="I2" s="14">
         <v>0</v>
       </c>
     </row>
@@ -3360,28 +3317,28 @@
       <c r="A3" s="6">
         <v>3000000</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="14">
         <v>46200</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="14">
         <v>64680</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="14">
         <v>83160</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="14">
         <v>101640</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="14">
         <v>120120</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="14">
         <v>141480</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="14">
         <v>162840</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="14">
         <v>0</v>
       </c>
     </row>
@@ -3389,28 +3346,28 @@
       <c r="A4" s="6">
         <v>2500000</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="14">
         <v>44400</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="14">
         <v>62160</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="14">
         <v>79920</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="14">
         <v>97680</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="14">
         <v>115440</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="14">
         <v>133200</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="14">
         <v>150960</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="14">
         <v>0</v>
       </c>
     </row>
@@ -3418,28 +3375,28 @@
       <c r="A5" s="6">
         <v>2000000</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="14">
         <v>38400</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="14">
         <v>53760</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
         <v>69120</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>84480</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="14">
         <v>99840</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="14">
         <v>115200</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="14">
         <v>130560</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="14">
         <v>0</v>
       </c>
     </row>
@@ -3447,28 +3404,28 @@
       <c r="A6" s="6">
         <v>1500000</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>32400</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="14">
         <v>45360</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <v>58320</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <v>71280</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="14">
         <v>84240</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="14">
         <v>97200</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="14">
         <v>110160</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="14">
         <v>0</v>
       </c>
     </row>
@@ -3476,28 +3433,28 @@
       <c r="A7" s="6">
         <v>1000000</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="14">
         <v>26400</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="14">
         <v>36960</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <v>47520</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <v>58080</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="14">
         <v>68640</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="14">
         <v>79200</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="14">
         <v>89760</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="14">
         <v>0</v>
       </c>
     </row>
@@ -3505,28 +3462,28 @@
       <c r="A8" s="6">
         <v>750000</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>23400</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="14">
         <v>32760</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="14">
         <v>42120</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <v>51480</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="14">
         <v>60840</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="14">
         <v>70200</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="14">
         <v>79560</v>
       </c>
-      <c r="I8" s="15">
+      <c r="I8" s="14">
         <v>0</v>
       </c>
     </row>
@@ -3534,28 +3491,28 @@
       <c r="A9" s="6">
         <v>500000</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="14">
         <v>20400</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="14">
         <v>28560</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <v>36720</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="14">
         <v>44880</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="14">
         <v>53040</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="14">
         <v>61200</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="14">
         <v>69360</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="14">
         <v>0</v>
       </c>
     </row>
@@ -3563,28 +3520,28 @@
       <c r="A10" s="6">
         <v>300000</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="14">
         <v>18000</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="14">
         <v>25200</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="14">
         <v>32400</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="14">
         <v>39600</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="14">
         <v>46800</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="14">
         <v>54000</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="14">
         <v>61200</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="14">
         <v>0</v>
       </c>
     </row>
@@ -3592,28 +3549,28 @@
       <c r="A11" s="6">
         <v>200000</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="14">
         <v>16800</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="14">
         <v>23520</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="14">
         <v>30240</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="14">
         <v>36960</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="14">
         <v>43680</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="14">
         <v>50400</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="14">
         <v>57120</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="14">
         <v>0</v>
       </c>
     </row>
@@ -3629,247 +3586,247 @@
   </sheetPr>
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="18" customWidth="1"/>
-    <col min="2" max="7" width="10" style="18" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="18" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" style="17" customWidth="1"/>
+    <col min="2" max="7" width="10" style="17" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="17" customWidth="1"/>
     <col min="9" max="10" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="35" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="34" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="19" customFormat="1" ht="14.25" collapsed="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17">
+    </row>
+    <row r="2" spans="1:9" s="18" customFormat="1" ht="14.25" collapsed="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="16">
         <v>250000</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="14">
         <v>54600</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="14">
         <v>65520</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="14">
         <v>76440</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="14">
         <v>87360</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="14">
         <v>98280</v>
       </c>
-      <c r="G2" s="15">
+      <c r="G2" s="14">
         <v>109200</v>
       </c>
-      <c r="H2" s="15">
+      <c r="H2" s="14">
         <v>120120</v>
       </c>
-      <c r="I2" s="15">
+      <c r="I2" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17">
+      <c r="A3" s="16">
         <v>200000</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="14">
         <v>45600</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="14">
         <v>56520</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="14">
         <v>67440</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="14">
         <v>78360</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="14">
         <v>89280</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="14">
         <v>100200</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="14">
         <v>111120</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
+      <c r="A4" s="16">
         <v>150000</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="14">
         <v>36600</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="14">
         <v>47520</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="14">
         <v>58440</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="14">
         <v>69360</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="14">
         <v>80280</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="14">
         <v>91200</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="14">
         <v>102120</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
+      <c r="A5" s="16">
         <v>100000</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="14">
         <v>27600</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="14">
         <v>38520</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
         <v>49440</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>60360</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="14">
         <v>71280</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="14">
         <v>82200</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="14">
         <v>93120</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
+      <c r="A6" s="16">
         <v>75000</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>23100</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="14">
         <v>34020</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <v>44940</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <v>55860</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="14">
         <v>66780</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="14">
         <v>66780</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="14">
         <v>66780</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
+      <c r="A7" s="16">
         <v>50000</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="14">
         <v>18600</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="14">
         <v>29520</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <v>40440</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <v>40440</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="14">
         <v>40440</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="14">
         <v>40440</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="14">
         <v>40440</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
+      <c r="A8" s="16">
         <v>40000</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>16800</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="14">
         <v>27720</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="14">
         <v>38640</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <v>38640</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="14">
         <v>38640</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="14">
         <v>38640</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="14">
         <v>38640</v>
       </c>
-      <c r="I8" s="15">
+      <c r="I8" s="14">
         <v>0</v>
       </c>
     </row>
@@ -3982,270 +3939,247 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84DFDA4-308E-451B-BDBF-3CACB189D037}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="I1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="16">
+        <v>250000</v>
+      </c>
+      <c r="B2" s="14">
+        <v>62790</v>
+      </c>
+      <c r="C2" s="14">
+        <v>75348</v>
+      </c>
+      <c r="D2" s="14">
+        <v>87906</v>
+      </c>
+      <c r="E2" s="14">
+        <v>100464</v>
+      </c>
+      <c r="F2" s="14">
+        <v>113022</v>
+      </c>
+      <c r="G2" s="14">
+        <v>125580</v>
+      </c>
+      <c r="H2" s="14">
+        <v>138138</v>
+      </c>
+      <c r="I2" s="14">
         <v>0</v>
       </c>
-      <c r="B2" s="17">
-        <v>250000</v>
-      </c>
-      <c r="C2" s="15">
-        <v>62790</v>
-      </c>
-      <c r="D2" s="15">
-        <v>75348</v>
-      </c>
-      <c r="E2" s="15">
-        <v>87906</v>
-      </c>
-      <c r="F2" s="15">
-        <v>100464</v>
-      </c>
-      <c r="G2" s="15">
-        <v>113022</v>
-      </c>
-      <c r="H2" s="15">
-        <v>125580</v>
-      </c>
-      <c r="I2" s="15">
-        <v>138138</v>
-      </c>
-      <c r="J2" s="15">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
+        <v>200000</v>
+      </c>
+      <c r="B3" s="14">
+        <v>52440</v>
+      </c>
+      <c r="C3" s="14">
+        <v>64998</v>
+      </c>
+      <c r="D3" s="14">
+        <v>77556</v>
+      </c>
+      <c r="E3" s="14">
+        <v>90114</v>
+      </c>
+      <c r="F3" s="14">
+        <v>102672</v>
+      </c>
+      <c r="G3" s="14">
+        <v>115230</v>
+      </c>
+      <c r="H3" s="14">
+        <v>127788</v>
+      </c>
+      <c r="I3" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="17">
-        <v>200000</v>
-      </c>
-      <c r="C3" s="15">
-        <v>52440</v>
-      </c>
-      <c r="D3" s="15">
-        <v>64998</v>
-      </c>
-      <c r="E3" s="15">
-        <v>77556</v>
-      </c>
-      <c r="F3" s="15">
-        <v>90114</v>
-      </c>
-      <c r="G3" s="15">
-        <v>102672</v>
-      </c>
-      <c r="H3" s="15">
-        <v>115230</v>
-      </c>
-      <c r="I3" s="15">
-        <v>127788</v>
-      </c>
-      <c r="J3" s="15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <v>150000</v>
+      </c>
+      <c r="B4" s="14">
+        <v>42090</v>
+      </c>
+      <c r="C4" s="14">
+        <v>54648</v>
+      </c>
+      <c r="D4" s="14">
+        <v>67206</v>
+      </c>
+      <c r="E4" s="14">
+        <v>79764</v>
+      </c>
+      <c r="F4" s="14">
+        <v>92322</v>
+      </c>
+      <c r="G4" s="14">
+        <v>104880</v>
+      </c>
+      <c r="H4" s="14">
+        <v>117438</v>
+      </c>
+      <c r="I4" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="17">
-        <v>150000</v>
-      </c>
-      <c r="C4" s="15">
-        <v>42090</v>
-      </c>
-      <c r="D4" s="15">
-        <v>54648</v>
-      </c>
-      <c r="E4" s="15">
-        <v>67206</v>
-      </c>
-      <c r="F4" s="15">
-        <v>79764</v>
-      </c>
-      <c r="G4" s="15">
-        <v>92322</v>
-      </c>
-      <c r="H4" s="15">
-        <v>104880</v>
-      </c>
-      <c r="I4" s="15">
-        <v>117438</v>
-      </c>
-      <c r="J4" s="15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
+        <v>100000</v>
+      </c>
+      <c r="B5" s="14">
+        <v>31740</v>
+      </c>
+      <c r="C5" s="14">
+        <v>44298</v>
+      </c>
+      <c r="D5" s="14">
+        <v>56856</v>
+      </c>
+      <c r="E5" s="14">
+        <v>69414</v>
+      </c>
+      <c r="F5" s="14">
+        <v>81972</v>
+      </c>
+      <c r="G5" s="14">
+        <v>94530</v>
+      </c>
+      <c r="H5" s="14">
+        <v>107088</v>
+      </c>
+      <c r="I5" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="17">
-        <v>100000</v>
-      </c>
-      <c r="C5" s="15">
-        <v>31740</v>
-      </c>
-      <c r="D5" s="15">
-        <v>44298</v>
-      </c>
-      <c r="E5" s="15">
-        <v>56856</v>
-      </c>
-      <c r="F5" s="15">
-        <v>69414</v>
-      </c>
-      <c r="G5" s="15">
-        <v>81972</v>
-      </c>
-      <c r="H5" s="15">
-        <v>94530</v>
-      </c>
-      <c r="I5" s="15">
-        <v>107088</v>
-      </c>
-      <c r="J5" s="15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="16">
+        <v>75000</v>
+      </c>
+      <c r="B6" s="14">
+        <v>26565</v>
+      </c>
+      <c r="C6" s="14">
+        <v>39123</v>
+      </c>
+      <c r="D6" s="14">
+        <v>51681</v>
+      </c>
+      <c r="E6" s="14">
+        <v>64239</v>
+      </c>
+      <c r="F6" s="14">
+        <v>76797</v>
+      </c>
+      <c r="G6" s="14">
+        <v>76797</v>
+      </c>
+      <c r="H6" s="14">
+        <v>76797</v>
+      </c>
+      <c r="I6" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="17">
-        <v>75000</v>
-      </c>
-      <c r="C6" s="15">
-        <v>26565</v>
-      </c>
-      <c r="D6" s="15">
-        <v>39123</v>
-      </c>
-      <c r="E6" s="15">
-        <v>51681</v>
-      </c>
-      <c r="F6" s="15">
-        <v>64239</v>
-      </c>
-      <c r="G6" s="15">
-        <v>76797</v>
-      </c>
-      <c r="H6" s="15">
-        <v>76797</v>
-      </c>
-      <c r="I6" s="15">
-        <v>76797</v>
-      </c>
-      <c r="J6" s="15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
+        <v>50000</v>
+      </c>
+      <c r="B7" s="14">
+        <v>21390</v>
+      </c>
+      <c r="C7" s="14">
+        <v>33948</v>
+      </c>
+      <c r="D7" s="14">
+        <v>46506</v>
+      </c>
+      <c r="E7" s="14">
+        <v>46506</v>
+      </c>
+      <c r="F7" s="14">
+        <v>46506</v>
+      </c>
+      <c r="G7" s="14">
+        <v>46506</v>
+      </c>
+      <c r="H7" s="14">
+        <v>46506</v>
+      </c>
+      <c r="I7" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="17">
-        <v>50000</v>
-      </c>
-      <c r="C7" s="15">
-        <v>21390</v>
-      </c>
-      <c r="D7" s="15">
-        <v>33948</v>
-      </c>
-      <c r="E7" s="15">
-        <v>46506</v>
-      </c>
-      <c r="F7" s="15">
-        <v>46506</v>
-      </c>
-      <c r="G7" s="15">
-        <v>46506</v>
-      </c>
-      <c r="H7" s="15">
-        <v>46506</v>
-      </c>
-      <c r="I7" s="15">
-        <v>46506</v>
-      </c>
-      <c r="J7" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="17">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
         <v>40000</v>
       </c>
-      <c r="C8" s="15">
+      <c r="B8" s="14">
         <v>19320</v>
       </c>
-      <c r="D8" s="15">
+      <c r="C8" s="14">
         <v>31878</v>
       </c>
-      <c r="E8" s="15">
+      <c r="D8" s="14">
         <v>44436</v>
       </c>
-      <c r="F8" s="15">
+      <c r="E8" s="14">
         <v>44436</v>
       </c>
-      <c r="G8" s="15">
+      <c r="F8" s="14">
         <v>44436</v>
       </c>
-      <c r="H8" s="15">
+      <c r="G8" s="14">
         <v>44436</v>
       </c>
-      <c r="I8" s="15">
+      <c r="H8" s="14">
         <v>44436</v>
       </c>
-      <c r="J8" s="15">
+      <c r="I8" s="14">
         <v>0</v>
       </c>
     </row>
@@ -4261,7 +4195,7 @@
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -4276,256 +4210,256 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="38" t="s">
-        <v>15</v>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>7</v>
       </c>
       <c r="I1" s="12"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="21">
+      <c r="A2" s="20">
         <v>10000</v>
       </c>
-      <c r="B2" s="23">
+      <c r="B2" s="22">
         <v>3250</v>
       </c>
-      <c r="C2" s="23">
+      <c r="C2" s="22">
         <v>4250</v>
       </c>
-      <c r="D2" s="23">
+      <c r="D2" s="22">
         <v>4750</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="22">
         <v>5250</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="22">
         <v>5750</v>
       </c>
-      <c r="G2" s="23">
+      <c r="G2" s="22">
         <v>6750</v>
       </c>
-      <c r="H2" s="25">
+      <c r="H2" s="24">
         <v>1012.5</v>
       </c>
       <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="20">
+      <c r="A3" s="19">
         <v>20000</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="22">
         <v>6500</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="22">
         <v>8500</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="22">
         <v>9500</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="22">
         <v>10500</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="22">
         <v>11500</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="22">
         <v>13500</v>
       </c>
-      <c r="H3" s="25">
+      <c r="H3" s="24">
         <v>2025</v>
       </c>
       <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="20">
+      <c r="A4" s="19">
         <v>25000</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4" s="22">
         <v>8125</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="22">
         <v>10625</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="22">
         <v>11875</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="22">
         <v>13125</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="22">
         <v>14375</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="22">
         <v>16875</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="24">
         <v>2531.25</v>
       </c>
       <c r="I4" s="12"/>
-      <c r="L4" s="33"/>
+      <c r="L4" s="32"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="20">
+      <c r="A5" s="19">
         <v>30000</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B5" s="22">
         <v>9750</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="22">
         <v>12750</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="22">
         <v>14250</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="22">
         <v>15750</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="22">
         <v>17250</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="22">
         <v>20250</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="24">
         <v>3037.5</v>
       </c>
       <c r="I5" s="12"/>
-      <c r="L5" s="33"/>
+      <c r="L5" s="32"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="20">
+      <c r="A6" s="19">
         <v>35000</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6" s="22">
         <v>11375</v>
       </c>
-      <c r="C6" s="23">
+      <c r="C6" s="22">
         <v>14875</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="22">
         <v>16625</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="22">
         <v>18375</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="22">
         <v>20125</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="22">
         <v>23625</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="24">
         <v>3543.75</v>
       </c>
       <c r="I6" s="12"/>
-      <c r="L6" s="33"/>
+      <c r="L6" s="32"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="20">
+      <c r="A7" s="19">
         <v>40000</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B7" s="22">
         <v>13000</v>
       </c>
-      <c r="C7" s="23">
+      <c r="C7" s="22">
         <v>17000</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="22">
         <v>19000</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="22">
         <v>21000</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="22">
         <v>23000</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="22">
         <v>27000</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="24">
         <v>4050</v>
       </c>
       <c r="I7" s="12"/>
-      <c r="L7" s="33"/>
+      <c r="L7" s="32"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="20">
+      <c r="A8" s="19">
         <v>45000</v>
       </c>
-      <c r="B8" s="23">
+      <c r="B8" s="22">
         <v>14625</v>
       </c>
-      <c r="C8" s="23">
+      <c r="C8" s="22">
         <v>19125</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="22">
         <v>21375</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="22">
         <v>23625</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="22">
         <v>25875</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G8" s="22">
         <v>30375</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="24">
         <v>4556.25</v>
       </c>
       <c r="I8" s="12"/>
-      <c r="L8" s="33"/>
+      <c r="L8" s="32"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="20">
+      <c r="A9" s="19">
         <v>50000</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="22">
         <v>16250</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="22">
         <v>21250</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="22">
         <v>23750</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="22">
         <v>26250</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="22">
         <v>28750</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="22">
         <v>33750</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="24">
         <v>5062.5</v>
       </c>
       <c r="I9" s="12"/>
-      <c r="L9" s="33"/>
+      <c r="L9" s="32"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L10" s="33"/>
+      <c r="L10" s="32"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -4545,234 +4479,234 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20">
+        <v>10000</v>
+      </c>
+      <c r="C1" s="20">
+        <v>20000</v>
+      </c>
+      <c r="D1" s="20">
+        <v>25000</v>
+      </c>
+      <c r="E1" s="20">
+        <v>30000</v>
+      </c>
+      <c r="F1" s="20">
+        <v>35000</v>
+      </c>
+      <c r="G1" s="20">
+        <v>40000</v>
+      </c>
+      <c r="H1" s="20">
+        <v>45000</v>
+      </c>
+      <c r="I1" s="20">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="22">
+        <v>3250</v>
+      </c>
+      <c r="C2" s="22">
+        <v>6500</v>
+      </c>
+      <c r="D2" s="22">
+        <v>8125</v>
+      </c>
+      <c r="E2" s="22">
+        <v>9750</v>
+      </c>
+      <c r="F2" s="22">
+        <v>11375</v>
+      </c>
+      <c r="G2" s="22">
+        <v>13000</v>
+      </c>
+      <c r="H2" s="22">
+        <v>14625</v>
+      </c>
+      <c r="I2" s="22">
+        <v>16250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="22">
+        <v>4250</v>
+      </c>
+      <c r="C3" s="22">
+        <v>8500</v>
+      </c>
+      <c r="D3" s="22">
+        <v>10625</v>
+      </c>
+      <c r="E3" s="22">
+        <v>12750</v>
+      </c>
+      <c r="F3" s="22">
+        <v>14875</v>
+      </c>
+      <c r="G3" s="22">
+        <v>17000</v>
+      </c>
+      <c r="H3" s="22">
+        <v>19125</v>
+      </c>
+      <c r="I3" s="22">
+        <v>21250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="22">
+        <v>4750</v>
+      </c>
+      <c r="C4" s="22">
+        <v>9500</v>
+      </c>
+      <c r="D4" s="22">
+        <v>11875</v>
+      </c>
+      <c r="E4" s="22">
+        <v>14250</v>
+      </c>
+      <c r="F4" s="22">
+        <v>16625</v>
+      </c>
+      <c r="G4" s="22">
+        <v>19000</v>
+      </c>
+      <c r="H4" s="22">
+        <v>21375</v>
+      </c>
+      <c r="I4" s="22">
+        <v>23750</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="22">
+        <v>5250</v>
+      </c>
+      <c r="C5" s="22">
+        <v>10500</v>
+      </c>
+      <c r="D5" s="22">
+        <v>13125</v>
+      </c>
+      <c r="E5" s="22">
+        <v>15750</v>
+      </c>
+      <c r="F5" s="22">
+        <v>18375</v>
+      </c>
+      <c r="G5" s="22">
+        <v>21000</v>
+      </c>
+      <c r="H5" s="22">
+        <v>23625</v>
+      </c>
+      <c r="I5" s="22">
+        <v>26250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="22">
+        <v>5750</v>
+      </c>
+      <c r="C6" s="22">
+        <v>11500</v>
+      </c>
+      <c r="D6" s="22">
+        <v>14375</v>
+      </c>
+      <c r="E6" s="22">
+        <v>17250</v>
+      </c>
+      <c r="F6" s="22">
+        <v>20125</v>
+      </c>
+      <c r="G6" s="22">
+        <v>23000</v>
+      </c>
+      <c r="H6" s="22">
+        <v>25875</v>
+      </c>
+      <c r="I6" s="22">
+        <v>28750</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="22">
+        <v>6750</v>
+      </c>
+      <c r="C7" s="22">
+        <v>13500</v>
+      </c>
+      <c r="D7" s="22">
+        <v>16875</v>
+      </c>
+      <c r="E7" s="22">
+        <v>20250</v>
+      </c>
+      <c r="F7" s="22">
+        <v>23625</v>
+      </c>
+      <c r="G7" s="22">
+        <v>27000</v>
+      </c>
+      <c r="H7" s="22">
+        <v>30375</v>
+      </c>
+      <c r="I7" s="22">
+        <v>33750</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="21">
-        <v>10000</v>
-      </c>
-      <c r="C1" s="21">
-        <v>20000</v>
-      </c>
-      <c r="D1" s="21">
-        <v>25000</v>
-      </c>
-      <c r="E1" s="21">
-        <v>30000</v>
-      </c>
-      <c r="F1" s="21">
-        <v>35000</v>
-      </c>
-      <c r="G1" s="21">
-        <v>40000</v>
-      </c>
-      <c r="H1" s="21">
-        <v>45000</v>
-      </c>
-      <c r="I1" s="21">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="23">
-        <v>3250</v>
-      </c>
-      <c r="C2" s="23">
-        <v>6500</v>
-      </c>
-      <c r="D2" s="23">
-        <v>8125</v>
-      </c>
-      <c r="E2" s="23">
-        <v>9750</v>
-      </c>
-      <c r="F2" s="23">
-        <v>11375</v>
-      </c>
-      <c r="G2" s="23">
-        <v>13000</v>
-      </c>
-      <c r="H2" s="23">
-        <v>14625</v>
-      </c>
-      <c r="I2" s="23">
-        <v>16250</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="23">
-        <v>4250</v>
-      </c>
-      <c r="C3" s="23">
-        <v>8500</v>
-      </c>
-      <c r="D3" s="23">
-        <v>10625</v>
-      </c>
-      <c r="E3" s="23">
-        <v>12750</v>
-      </c>
-      <c r="F3" s="23">
-        <v>14875</v>
-      </c>
-      <c r="G3" s="23">
-        <v>17000</v>
-      </c>
-      <c r="H3" s="23">
-        <v>19125</v>
-      </c>
-      <c r="I3" s="23">
-        <v>21250</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="23">
-        <v>4750</v>
-      </c>
-      <c r="C4" s="23">
-        <v>9500</v>
-      </c>
-      <c r="D4" s="23">
-        <v>11875</v>
-      </c>
-      <c r="E4" s="23">
-        <v>14250</v>
-      </c>
-      <c r="F4" s="23">
-        <v>16625</v>
-      </c>
-      <c r="G4" s="23">
-        <v>19000</v>
-      </c>
-      <c r="H4" s="23">
-        <v>21375</v>
-      </c>
-      <c r="I4" s="23">
-        <v>23750</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="23">
-        <v>5250</v>
-      </c>
-      <c r="C5" s="23">
-        <v>10500</v>
-      </c>
-      <c r="D5" s="23">
-        <v>13125</v>
-      </c>
-      <c r="E5" s="23">
-        <v>15750</v>
-      </c>
-      <c r="F5" s="23">
-        <v>18375</v>
-      </c>
-      <c r="G5" s="23">
-        <v>21000</v>
-      </c>
-      <c r="H5" s="23">
-        <v>23625</v>
-      </c>
-      <c r="I5" s="23">
-        <v>26250</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="23">
-        <v>5750</v>
-      </c>
-      <c r="C6" s="23">
-        <v>11500</v>
-      </c>
-      <c r="D6" s="23">
-        <v>14375</v>
-      </c>
-      <c r="E6" s="23">
-        <v>17250</v>
-      </c>
-      <c r="F6" s="23">
-        <v>20125</v>
-      </c>
-      <c r="G6" s="23">
-        <v>23000</v>
-      </c>
-      <c r="H6" s="23">
-        <v>25875</v>
-      </c>
-      <c r="I6" s="23">
-        <v>28750</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="23">
-        <v>6750</v>
-      </c>
-      <c r="C7" s="23">
-        <v>13500</v>
-      </c>
-      <c r="D7" s="23">
-        <v>16875</v>
-      </c>
-      <c r="E7" s="23">
-        <v>20250</v>
-      </c>
-      <c r="F7" s="23">
-        <v>23625</v>
-      </c>
-      <c r="G7" s="23">
-        <v>27000</v>
-      </c>
-      <c r="H7" s="23">
-        <v>30375</v>
-      </c>
-      <c r="I7" s="23">
-        <v>33750</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="25">
+      <c r="B8" s="24">
         <v>1012.5</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="24">
         <v>2025</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="24">
         <v>2531.25</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="24">
         <v>3037.5</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="24">
         <v>3543.75</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="24">
         <v>4050</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="24">
         <v>4556.25</v>
       </c>
-      <c r="I8" s="25">
+      <c r="I8" s="24">
         <v>5062.5</v>
       </c>
     </row>
@@ -4798,59 +4732,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>17</v>
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="27">
+      <c r="A2" s="26">
         <v>50000</v>
       </c>
-      <c r="B2" s="28">
+      <c r="B2" s="27">
         <v>10631.25</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="27">
+      <c r="A3" s="26">
         <v>75000</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="27">
         <v>15947</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="27">
+      <c r="A4" s="26">
         <v>100000</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="27">
         <v>21262.5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="27">
+      <c r="A5" s="26">
         <v>150000</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="27">
         <v>31893.75</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="27">
+      <c r="A6" s="26">
         <v>200000</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="27">
         <v>42525</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D7" s="33"/>
-      <c r="F7" s="33"/>
+      <c r="D7" s="32"/>
+      <c r="F7" s="32"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="33"/>
+      <c r="B9" s="32"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>